<commit_message>
enable headless and adding new features in extend
</commit_message>
<xml_diff>
--- a/ExcelFileData/WriteItemData.xlsx
+++ b/ExcelFileData/WriteItemData.xlsx
@@ -12,36 +12,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Zebronics - Wireless Bluetooth Headset</t>
   </si>
   <si>
-    <t>Rs. 949</t>
+    <t>Rs. 847</t>
   </si>
   <si>
-    <t>boAt Rockerz 261 In Ear Wireless With Mic Headphones/Earphones (Blue)</t>
+    <t>TUNE AUDIO U&amp;I NICE Neckband Wireless With Mic Headphones/Earphones Beige and Black</t>
   </si>
   <si>
-    <t>Rs. 1,189</t>
+    <t>Rs. 749</t>
   </si>
   <si>
-    <t>hitage Tws-68 Bella Series In Ear True Wireless (TWS) 5 Hours Playback IPX4(Splash &amp; Sweat Proof) Auto pairLight weight -Bluetooth V 5.3 Royal Blue</t>
+    <t>NBOX STAR WIRELESS NECKBAND WITH DOLBY EFFECT BASS SOUND IPX5 WITH MASSIVE MUSIC PLAYBACK WITH 1 YEAR WARRANTY BLUETOOTH HEADPHONE,BLUETOOTH EARPHONE,BLUETOOTH NECKBAND</t>
   </si>
   <si>
-    <t>Rs. 899</t>
-  </si>
-  <si>
-    <t>NBOX Gaming TWS Earbuds Ear Buds Wireless Ear Buds Wireless With Mic Headphones/Earphones Black</t>
+    <t>NBOX INVICTUS Neckband Wireless With Mic Headphones/Earphones Gold</t>
   </si>
   <si>
     <t>Rs. 999</t>
   </si>
   <si>
-    <t>hitage NBT-6767 + [ 38 HOURS PLAYTIME ] Bluetooth Headphone/ Neckband Wireless With Mic Headphones/Earphones Red Cream</t>
+    <t>boAt Airdopes 131/138 On Ear True Wireless (TWS) 15 Hours Playback IPX7(Water Resistant) Active Noise cancellation -Bluetooth V 5.0 Black</t>
   </si>
   <si>
-    <t>Rs. 799</t>
+    <t>Rs. 1,299</t>
   </si>
 </sst>
 </file>
@@ -113,23 +110,23 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>